<commit_message>
Script to handle admin pages in LiveSLR
</commit_message>
<xml_diff>
--- a/Testdata/DataFile_AdminPage_Testing.xlsx
+++ b/Testdata/DataFile_AdminPage_Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AFD6C5-D438-4DF4-AE56-AAA18CFEB523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6D61C8-CA84-4C5D-B71D-92167F9033EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>This population is being created by Script for validation</t>
   </si>
@@ -46,12 +46,6 @@
     <t>Pfizer-Economic-Report-20220725120854.xlsx</t>
   </si>
   <si>
-    <t>D:\\VersionControl\\pse.autotest\\ExtractionTemplate\\Pfizer-Economic-Report-20220725120854.xlsx</t>
-  </si>
-  <si>
-    <t>D:\\VersionControl\\pse.autotest\\ExtractionTemplate\\sample_population_data_sheet.xlsx</t>
-  </si>
-  <si>
     <t>Expected_File_names</t>
   </si>
   <si>
@@ -85,34 +79,10 @@
     <t>X_Automation_Test</t>
   </si>
   <si>
-    <t>Interventional</t>
-  </si>
-  <si>
-    <t>Economic</t>
-  </si>
-  <si>
-    <t>Quality of life</t>
-  </si>
-  <si>
-    <t>Real-world Evidence</t>
-  </si>
-  <si>
-    <t>Study_Types</t>
-  </si>
-  <si>
-    <t>QA_Excel_Files</t>
-  </si>
-  <si>
-    <t>D:\\VersionControl\\pse.autotest\\ExtractionTemplate\\sample_population_data_sheet - Copy (1).xlsx</t>
-  </si>
-  <si>
-    <t>D:\\VersionControl\\pse.autotest\\ExtractionTemplate\\sample_population_data_sheet - Copy (2).xlsx</t>
-  </si>
-  <si>
-    <t>D:\\VersionControl\\pse.autotest\\ExtractionTemplate\\sample_population_data_sheet - Copy (3).xlsx</t>
-  </si>
-  <si>
-    <t>D:\\VersionControl\\pse.autotest\\ExtractionTemplate\\sample_population_data_sheet - Copy (4).xlsx</t>
+    <t>\ExtractionTemplate\sample_population_data_sheet.xlsx</t>
+  </si>
+  <si>
+    <t>\ExtractionTemplate\Pfizer-Economic-Report-20220725120854.xlsx</t>
   </si>
 </sst>
 </file>
@@ -151,11 +121,9 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,114 +404,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="24.44140625" style="1"/>
-    <col min="5" max="5" width="28.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="24.44140625" style="1"/>
+    <col min="1" max="1" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="57.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="24.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
+      <c r="E3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the script to create test.log file if not exist
</commit_message>
<xml_diff>
--- a/Testdata/DataFile_AdminPage_Testing.xlsx
+++ b/Testdata/DataFile_AdminPage_Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6D61C8-CA84-4C5D-B71D-92167F9033EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3BA9DD-CC96-4A0C-AEC3-10AC7D71D772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,17 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>This population is being created by Script for validation</t>
   </si>
   <si>
-    <t>sample_population_data_sheet.xlsx</t>
-  </si>
-  <si>
-    <t>Pfizer-Economic-Report-20220725120854.xlsx</t>
-  </si>
-  <si>
     <t>Expected_File_names</t>
   </si>
   <si>
@@ -79,10 +73,22 @@
     <t>X_Automation_Test</t>
   </si>
   <si>
-    <t>\ExtractionTemplate\sample_population_data_sheet.xlsx</t>
-  </si>
-  <si>
-    <t>\ExtractionTemplate\Pfizer-Economic-Report-20220725120854.xlsx</t>
+    <t>\ExtractionTemplate\ImportPublications\IC AML - Success Case Sheet.xlsx</t>
+  </si>
+  <si>
+    <t>\ExtractionTemplate\ImportPublications\ICER - Failure Case Sheet.xlsx</t>
+  </si>
+  <si>
+    <t>ICER - Failure Case Sheet.xlsx</t>
+  </si>
+  <si>
+    <t>IC AML - Success Case Sheet.xlsx</t>
+  </si>
+  <si>
+    <t>\ExtractionTemplate\extraction-template.xlsx</t>
+  </si>
+  <si>
+    <t>extraction-template.xlsx</t>
   </si>
 </sst>
 </file>
@@ -407,7 +413,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -415,7 +421,7 @@
     <col min="1" max="1" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="57.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="24.44140625" style="2"/>
@@ -423,61 +429,61 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>0</v>

</xml_diff>